<commit_message>
1 Asset working to 9th level: Fixed indexing of arrays in thrust functors
</commit_message>
<xml_diff>
--- a/SparseGridCollocation/GenerateCudaTestCode.xlsx
+++ b/SparseGridCollocation/GenerateCudaTestCode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Source\Repos\SparseGridCollocation2\SparseGridCollocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Source\Repos\SparseGridCollocation4\SparseGridCollocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22785,7 +22784,7 @@
     </row>
     <row r="137" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A137">
-        <f t="shared" ref="A137:A168" si="9">IF(A33&lt;&gt;A85,1,0)</f>
+        <f t="shared" ref="A137:A155" si="9">IF(A33&lt;&gt;A85,1,0)</f>
         <v>1</v>
       </c>
       <c r="B137">
@@ -37210,22 +37209,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B875B525-5D66-4742-AEC0-C579B8ABAACC}">
-  <dimension ref="B1:G195"/>
+  <dimension ref="B1:H195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G195"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H195" sqref="H1:H195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="str">
-        <f>_xlfn.CONCAT("TX1(",C1,",0","') = ",E1,";")</f>
-        <v>TX1(0,0') = 0;</v>
+        <f>_xlfn.CONCAT("TX1(",C1,",0",") = ",E1,";")</f>
+        <v>TX1(0,0) = 0;</v>
       </c>
       <c r="C1">
         <f>0</f>
@@ -37241,15 +37240,15 @@
       <c r="F1">
         <v>0</v>
       </c>
-      <c r="G1" t="str">
-        <f>_xlfn.CONCAT("TX1(",C1,",1","') = ",F1,";")</f>
-        <v>TX1(0,1') = 0;</v>
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT("TX1(",C1,",1",") = ",F1,";")</f>
+        <v>TX1(0,1) = 0;</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B65" si="0">_xlfn.CONCAT("TX1(",C2,",0","') = ",E2,";")</f>
-        <v>TX1(1,0') = 0;</v>
+        <f t="shared" ref="B2:B65" si="0">_xlfn.CONCAT("TX1(",C2,",0",") = ",E2,";")</f>
+        <v>TX1(1,0) = 0;</v>
       </c>
       <c r="C2">
         <f>C1+1</f>
@@ -37265,15 +37264,15 @@
       <c r="F2">
         <v>4.6875</v>
       </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G65" si="1">_xlfn.CONCAT("TX1(",C2,",1","') = ",F2,";")</f>
-        <v>TX1(1,1') = 4.6875;</v>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H65" si="1">_xlfn.CONCAT("TX1(",C2,",1",") = ",F2,";")</f>
+        <v>TX1(1,1) = 4.6875;</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(2,0') = 0;</v>
+        <v>TX1(2,0) = 0;</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="2">C2+1</f>
@@ -37289,15 +37288,15 @@
       <c r="F3">
         <v>9.375</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(2,1') = 9.375;</v>
+        <v>TX1(2,1) = 9.375;</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(3,0') = 0;</v>
+        <v>TX1(3,0) = 0;</v>
       </c>
       <c r="C4">
         <f t="shared" si="2"/>
@@ -37313,15 +37312,15 @@
       <c r="F4">
         <v>14.0625</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(3,1') = 14.0625;</v>
+        <v>TX1(3,1) = 14.0625;</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(4,0') = 0;</v>
+        <v>TX1(4,0) = 0;</v>
       </c>
       <c r="C5">
         <f t="shared" si="2"/>
@@ -37337,15 +37336,15 @@
       <c r="F5">
         <v>18.75</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(4,1') = 18.75;</v>
+        <v>TX1(4,1) = 18.75;</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(5,0') = 0;</v>
+        <v>TX1(5,0) = 0;</v>
       </c>
       <c r="C6">
         <f t="shared" si="2"/>
@@ -37361,15 +37360,15 @@
       <c r="F6">
         <v>23.4375</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(5,1') = 23.4375;</v>
+        <v>TX1(5,1) = 23.4375;</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(6,0') = 0;</v>
+        <v>TX1(6,0) = 0;</v>
       </c>
       <c r="C7">
         <f t="shared" si="2"/>
@@ -37385,15 +37384,15 @@
       <c r="F7">
         <v>28.125</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(6,1') = 28.125;</v>
+        <v>TX1(6,1) = 28.125;</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(7,0') = 0;</v>
+        <v>TX1(7,0) = 0;</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
@@ -37409,15 +37408,15 @@
       <c r="F8">
         <v>32.8125</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(7,1') = 32.8125;</v>
+        <v>TX1(7,1) = 32.8125;</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(8,0') = 0;</v>
+        <v>TX1(8,0) = 0;</v>
       </c>
       <c r="C9">
         <f t="shared" si="2"/>
@@ -37433,15 +37432,15 @@
       <c r="F9">
         <v>37.5</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(8,1') = 37.5;</v>
+        <v>TX1(8,1) = 37.5;</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(9,0') = 0;</v>
+        <v>TX1(9,0) = 0;</v>
       </c>
       <c r="C10">
         <f t="shared" si="2"/>
@@ -37457,15 +37456,15 @@
       <c r="F10">
         <v>42.1875</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(9,1') = 42.1875;</v>
+        <v>TX1(9,1) = 42.1875;</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(10,0') = 0;</v>
+        <v>TX1(10,0) = 0;</v>
       </c>
       <c r="C11">
         <f t="shared" si="2"/>
@@ -37481,15 +37480,15 @@
       <c r="F11">
         <v>46.875</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(10,1') = 46.875;</v>
+        <v>TX1(10,1) = 46.875;</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(11,0') = 0;</v>
+        <v>TX1(11,0) = 0;</v>
       </c>
       <c r="C12">
         <f t="shared" si="2"/>
@@ -37505,15 +37504,15 @@
       <c r="F12">
         <v>51.5625</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(11,1') = 51.5625;</v>
+        <v>TX1(11,1) = 51.5625;</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(12,0') = 0;</v>
+        <v>TX1(12,0) = 0;</v>
       </c>
       <c r="C13">
         <f t="shared" si="2"/>
@@ -37529,15 +37528,15 @@
       <c r="F13">
         <v>56.25</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(12,1') = 56.25;</v>
+        <v>TX1(12,1) = 56.25;</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(13,0') = 0;</v>
+        <v>TX1(13,0) = 0;</v>
       </c>
       <c r="C14">
         <f t="shared" si="2"/>
@@ -37553,15 +37552,15 @@
       <c r="F14">
         <v>60.9375</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(13,1') = 60.9375;</v>
+        <v>TX1(13,1) = 60.9375;</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(14,0') = 0;</v>
+        <v>TX1(14,0) = 0;</v>
       </c>
       <c r="C15">
         <f t="shared" si="2"/>
@@ -37577,15 +37576,15 @@
       <c r="F15">
         <v>65.625</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(14,1') = 65.625;</v>
+        <v>TX1(14,1) = 65.625;</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(15,0') = 0;</v>
+        <v>TX1(15,0) = 0;</v>
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
@@ -37601,15 +37600,15 @@
       <c r="F16">
         <v>70.3125</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(15,1') = 70.3125;</v>
+        <v>TX1(15,1) = 70.3125;</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(16,0') = 0;</v>
+        <v>TX1(16,0) = 0;</v>
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
@@ -37625,15 +37624,15 @@
       <c r="F17">
         <v>75</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(16,1') = 75;</v>
+        <v>TX1(16,1) = 75;</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(17,0') = 0;</v>
+        <v>TX1(17,0) = 0;</v>
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
@@ -37649,15 +37648,15 @@
       <c r="F18">
         <v>79.6875</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(17,1') = 79.6875;</v>
+        <v>TX1(17,1) = 79.6875;</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(18,0') = 0;</v>
+        <v>TX1(18,0) = 0;</v>
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
@@ -37673,15 +37672,15 @@
       <c r="F19">
         <v>84.375</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(18,1') = 84.375;</v>
+        <v>TX1(18,1) = 84.375;</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(19,0') = 0;</v>
+        <v>TX1(19,0) = 0;</v>
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
@@ -37697,15 +37696,15 @@
       <c r="F20">
         <v>89.0625</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(19,1') = 89.0625;</v>
+        <v>TX1(19,1) = 89.0625;</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(20,0') = 0;</v>
+        <v>TX1(20,0) = 0;</v>
       </c>
       <c r="C21">
         <f t="shared" si="2"/>
@@ -37721,15 +37720,15 @@
       <c r="F21">
         <v>93.75</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(20,1') = 93.75;</v>
+        <v>TX1(20,1) = 93.75;</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(21,0') = 0;</v>
+        <v>TX1(21,0) = 0;</v>
       </c>
       <c r="C22">
         <f t="shared" si="2"/>
@@ -37745,15 +37744,15 @@
       <c r="F22">
         <v>98.4375</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(21,1') = 98.4375;</v>
+        <v>TX1(21,1) = 98.4375;</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(22,0') = 0;</v>
+        <v>TX1(22,0) = 0;</v>
       </c>
       <c r="C23">
         <f t="shared" si="2"/>
@@ -37769,15 +37768,15 @@
       <c r="F23">
         <v>103.125</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(22,1') = 103.125;</v>
+        <v>TX1(22,1) = 103.125;</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(23,0') = 0;</v>
+        <v>TX1(23,0) = 0;</v>
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
@@ -37793,15 +37792,15 @@
       <c r="F24">
         <v>107.8125</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(23,1') = 107.8125;</v>
+        <v>TX1(23,1) = 107.8125;</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(24,0') = 0;</v>
+        <v>TX1(24,0) = 0;</v>
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
@@ -37817,15 +37816,15 @@
       <c r="F25">
         <v>112.5</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(24,1') = 112.5;</v>
+        <v>TX1(24,1) = 112.5;</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(25,0') = 0;</v>
+        <v>TX1(25,0) = 0;</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
@@ -37841,15 +37840,15 @@
       <c r="F26">
         <v>117.1875</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(25,1') = 117.1875;</v>
+        <v>TX1(25,1) = 117.1875;</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(26,0') = 0;</v>
+        <v>TX1(26,0) = 0;</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
@@ -37865,15 +37864,15 @@
       <c r="F27">
         <v>121.875</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(26,1') = 121.875;</v>
+        <v>TX1(26,1) = 121.875;</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(27,0') = 0;</v>
+        <v>TX1(27,0) = 0;</v>
       </c>
       <c r="C28">
         <f t="shared" si="2"/>
@@ -37889,15 +37888,15 @@
       <c r="F28">
         <v>126.5625</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(27,1') = 126.5625;</v>
+        <v>TX1(27,1) = 126.5625;</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(28,0') = 0;</v>
+        <v>TX1(28,0) = 0;</v>
       </c>
       <c r="C29">
         <f t="shared" si="2"/>
@@ -37913,15 +37912,15 @@
       <c r="F29">
         <v>131.25</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(28,1') = 131.25;</v>
+        <v>TX1(28,1) = 131.25;</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(29,0') = 0;</v>
+        <v>TX1(29,0) = 0;</v>
       </c>
       <c r="C30">
         <f t="shared" si="2"/>
@@ -37937,15 +37936,15 @@
       <c r="F30">
         <v>135.9375</v>
       </c>
-      <c r="G30" t="str">
+      <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(29,1') = 135.9375;</v>
+        <v>TX1(29,1) = 135.9375;</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(30,0') = 0;</v>
+        <v>TX1(30,0) = 0;</v>
       </c>
       <c r="C31">
         <f t="shared" si="2"/>
@@ -37961,15 +37960,15 @@
       <c r="F31">
         <v>140.625</v>
       </c>
-      <c r="G31" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(30,1') = 140.625;</v>
+        <v>TX1(30,1) = 140.625;</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(31,0') = 0;</v>
+        <v>TX1(31,0) = 0;</v>
       </c>
       <c r="C32">
         <f t="shared" si="2"/>
@@ -37985,15 +37984,15 @@
       <c r="F32">
         <v>145.3125</v>
       </c>
-      <c r="G32" t="str">
+      <c r="H32" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(31,1') = 145.3125;</v>
+        <v>TX1(31,1) = 145.3125;</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(32,0') = 0;</v>
+        <v>TX1(32,0) = 0;</v>
       </c>
       <c r="C33">
         <f t="shared" si="2"/>
@@ -38009,15 +38008,15 @@
       <c r="F33">
         <v>150</v>
       </c>
-      <c r="G33" t="str">
+      <c r="H33" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(32,1') = 150;</v>
+        <v>TX1(32,1) = 150;</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(33,0') = 0;</v>
+        <v>TX1(33,0) = 0;</v>
       </c>
       <c r="C34">
         <f t="shared" si="2"/>
@@ -38033,15 +38032,15 @@
       <c r="F34">
         <v>154.6875</v>
       </c>
-      <c r="G34" t="str">
+      <c r="H34" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(33,1') = 154.6875;</v>
+        <v>TX1(33,1) = 154.6875;</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(34,0') = 0;</v>
+        <v>TX1(34,0) = 0;</v>
       </c>
       <c r="C35">
         <f t="shared" si="2"/>
@@ -38057,15 +38056,15 @@
       <c r="F35">
         <v>159.375</v>
       </c>
-      <c r="G35" t="str">
+      <c r="H35" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(34,1') = 159.375;</v>
+        <v>TX1(34,1) = 159.375;</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(35,0') = 0;</v>
+        <v>TX1(35,0) = 0;</v>
       </c>
       <c r="C36">
         <f t="shared" si="2"/>
@@ -38081,15 +38080,15 @@
       <c r="F36">
         <v>164.0625</v>
       </c>
-      <c r="G36" t="str">
+      <c r="H36" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(35,1') = 164.0625;</v>
+        <v>TX1(35,1) = 164.0625;</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(36,0') = 0;</v>
+        <v>TX1(36,0) = 0;</v>
       </c>
       <c r="C37">
         <f t="shared" si="2"/>
@@ -38105,15 +38104,15 @@
       <c r="F37">
         <v>168.75</v>
       </c>
-      <c r="G37" t="str">
+      <c r="H37" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(36,1') = 168.75;</v>
+        <v>TX1(36,1) = 168.75;</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(37,0') = 0;</v>
+        <v>TX1(37,0) = 0;</v>
       </c>
       <c r="C38">
         <f t="shared" si="2"/>
@@ -38129,15 +38128,15 @@
       <c r="F38">
         <v>173.4375</v>
       </c>
-      <c r="G38" t="str">
+      <c r="H38" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(37,1') = 173.4375;</v>
+        <v>TX1(37,1) = 173.4375;</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(38,0') = 0;</v>
+        <v>TX1(38,0) = 0;</v>
       </c>
       <c r="C39">
         <f t="shared" si="2"/>
@@ -38153,15 +38152,15 @@
       <c r="F39">
         <v>178.125</v>
       </c>
-      <c r="G39" t="str">
+      <c r="H39" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(38,1') = 178.125;</v>
+        <v>TX1(38,1) = 178.125;</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(39,0') = 0;</v>
+        <v>TX1(39,0) = 0;</v>
       </c>
       <c r="C40">
         <f t="shared" si="2"/>
@@ -38177,15 +38176,15 @@
       <c r="F40">
         <v>182.8125</v>
       </c>
-      <c r="G40" t="str">
+      <c r="H40" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(39,1') = 182.8125;</v>
+        <v>TX1(39,1) = 182.8125;</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(40,0') = 0;</v>
+        <v>TX1(40,0) = 0;</v>
       </c>
       <c r="C41">
         <f t="shared" si="2"/>
@@ -38201,15 +38200,15 @@
       <c r="F41">
         <v>187.5</v>
       </c>
-      <c r="G41" t="str">
+      <c r="H41" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(40,1') = 187.5;</v>
+        <v>TX1(40,1) = 187.5;</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(41,0') = 0;</v>
+        <v>TX1(41,0) = 0;</v>
       </c>
       <c r="C42">
         <f t="shared" si="2"/>
@@ -38225,15 +38224,15 @@
       <c r="F42">
         <v>192.1875</v>
       </c>
-      <c r="G42" t="str">
+      <c r="H42" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(41,1') = 192.1875;</v>
+        <v>TX1(41,1) = 192.1875;</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(42,0') = 0;</v>
+        <v>TX1(42,0) = 0;</v>
       </c>
       <c r="C43">
         <f t="shared" si="2"/>
@@ -38249,15 +38248,15 @@
       <c r="F43">
         <v>196.875</v>
       </c>
-      <c r="G43" t="str">
+      <c r="H43" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(42,1') = 196.875;</v>
+        <v>TX1(42,1) = 196.875;</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(43,0') = 0;</v>
+        <v>TX1(43,0) = 0;</v>
       </c>
       <c r="C44">
         <f t="shared" si="2"/>
@@ -38273,15 +38272,15 @@
       <c r="F44">
         <v>201.5625</v>
       </c>
-      <c r="G44" t="str">
+      <c r="H44" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(43,1') = 201.5625;</v>
+        <v>TX1(43,1) = 201.5625;</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(44,0') = 0;</v>
+        <v>TX1(44,0) = 0;</v>
       </c>
       <c r="C45">
         <f t="shared" si="2"/>
@@ -38297,15 +38296,15 @@
       <c r="F45">
         <v>206.25</v>
       </c>
-      <c r="G45" t="str">
+      <c r="H45" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(44,1') = 206.25;</v>
+        <v>TX1(44,1) = 206.25;</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(45,0') = 0;</v>
+        <v>TX1(45,0) = 0;</v>
       </c>
       <c r="C46">
         <f t="shared" si="2"/>
@@ -38321,15 +38320,15 @@
       <c r="F46">
         <v>210.9375</v>
       </c>
-      <c r="G46" t="str">
+      <c r="H46" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(45,1') = 210.9375;</v>
+        <v>TX1(45,1) = 210.9375;</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(46,0') = 0;</v>
+        <v>TX1(46,0) = 0;</v>
       </c>
       <c r="C47">
         <f t="shared" si="2"/>
@@ -38345,15 +38344,15 @@
       <c r="F47">
         <v>215.625</v>
       </c>
-      <c r="G47" t="str">
+      <c r="H47" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(46,1') = 215.625;</v>
+        <v>TX1(46,1) = 215.625;</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(47,0') = 0;</v>
+        <v>TX1(47,0) = 0;</v>
       </c>
       <c r="C48">
         <f t="shared" si="2"/>
@@ -38369,15 +38368,15 @@
       <c r="F48">
         <v>220.3125</v>
       </c>
-      <c r="G48" t="str">
+      <c r="H48" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(47,1') = 220.3125;</v>
+        <v>TX1(47,1) = 220.3125;</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(48,0') = 0;</v>
+        <v>TX1(48,0) = 0;</v>
       </c>
       <c r="C49">
         <f t="shared" si="2"/>
@@ -38393,15 +38392,15 @@
       <c r="F49">
         <v>225</v>
       </c>
-      <c r="G49" t="str">
+      <c r="H49" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(48,1') = 225;</v>
+        <v>TX1(48,1) = 225;</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(49,0') = 0;</v>
+        <v>TX1(49,0) = 0;</v>
       </c>
       <c r="C50">
         <f t="shared" si="2"/>
@@ -38417,15 +38416,15 @@
       <c r="F50">
         <v>229.6875</v>
       </c>
-      <c r="G50" t="str">
+      <c r="H50" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(49,1') = 229.6875;</v>
+        <v>TX1(49,1) = 229.6875;</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(50,0') = 0;</v>
+        <v>TX1(50,0) = 0;</v>
       </c>
       <c r="C51">
         <f t="shared" si="2"/>
@@ -38441,15 +38440,15 @@
       <c r="F51">
         <v>234.375</v>
       </c>
-      <c r="G51" t="str">
+      <c r="H51" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(50,1') = 234.375;</v>
+        <v>TX1(50,1) = 234.375;</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(51,0') = 0;</v>
+        <v>TX1(51,0) = 0;</v>
       </c>
       <c r="C52">
         <f t="shared" si="2"/>
@@ -38465,15 +38464,15 @@
       <c r="F52">
         <v>239.0625</v>
       </c>
-      <c r="G52" t="str">
+      <c r="H52" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(51,1') = 239.0625;</v>
+        <v>TX1(51,1) = 239.0625;</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(52,0') = 0;</v>
+        <v>TX1(52,0) = 0;</v>
       </c>
       <c r="C53">
         <f t="shared" si="2"/>
@@ -38489,15 +38488,15 @@
       <c r="F53">
         <v>243.75</v>
       </c>
-      <c r="G53" t="str">
+      <c r="H53" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(52,1') = 243.75;</v>
+        <v>TX1(52,1) = 243.75;</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(53,0') = 0;</v>
+        <v>TX1(53,0) = 0;</v>
       </c>
       <c r="C54">
         <f t="shared" si="2"/>
@@ -38513,15 +38512,15 @@
       <c r="F54">
         <v>248.4375</v>
       </c>
-      <c r="G54" t="str">
+      <c r="H54" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(53,1') = 248.4375;</v>
+        <v>TX1(53,1) = 248.4375;</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(54,0') = 0;</v>
+        <v>TX1(54,0) = 0;</v>
       </c>
       <c r="C55">
         <f t="shared" si="2"/>
@@ -38537,15 +38536,15 @@
       <c r="F55">
         <v>253.125</v>
       </c>
-      <c r="G55" t="str">
+      <c r="H55" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(54,1') = 253.125;</v>
+        <v>TX1(54,1) = 253.125;</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(55,0') = 0;</v>
+        <v>TX1(55,0) = 0;</v>
       </c>
       <c r="C56">
         <f t="shared" si="2"/>
@@ -38561,15 +38560,15 @@
       <c r="F56">
         <v>257.8125</v>
       </c>
-      <c r="G56" t="str">
+      <c r="H56" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(55,1') = 257.8125;</v>
+        <v>TX1(55,1) = 257.8125;</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(56,0') = 0;</v>
+        <v>TX1(56,0) = 0;</v>
       </c>
       <c r="C57">
         <f t="shared" si="2"/>
@@ -38585,15 +38584,15 @@
       <c r="F57">
         <v>262.5</v>
       </c>
-      <c r="G57" t="str">
+      <c r="H57" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(56,1') = 262.5;</v>
+        <v>TX1(56,1) = 262.5;</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(57,0') = 0;</v>
+        <v>TX1(57,0) = 0;</v>
       </c>
       <c r="C58">
         <f t="shared" si="2"/>
@@ -38609,15 +38608,15 @@
       <c r="F58">
         <v>267.1875</v>
       </c>
-      <c r="G58" t="str">
+      <c r="H58" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(57,1') = 267.1875;</v>
+        <v>TX1(57,1) = 267.1875;</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(58,0') = 0;</v>
+        <v>TX1(58,0) = 0;</v>
       </c>
       <c r="C59">
         <f t="shared" si="2"/>
@@ -38633,15 +38632,15 @@
       <c r="F59">
         <v>271.875</v>
       </c>
-      <c r="G59" t="str">
+      <c r="H59" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(58,1') = 271.875;</v>
+        <v>TX1(58,1) = 271.875;</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(59,0') = 0;</v>
+        <v>TX1(59,0) = 0;</v>
       </c>
       <c r="C60">
         <f t="shared" si="2"/>
@@ -38657,15 +38656,15 @@
       <c r="F60">
         <v>276.5625</v>
       </c>
-      <c r="G60" t="str">
+      <c r="H60" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(59,1') = 276.5625;</v>
+        <v>TX1(59,1) = 276.5625;</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(60,0') = 0;</v>
+        <v>TX1(60,0) = 0;</v>
       </c>
       <c r="C61">
         <f t="shared" si="2"/>
@@ -38681,15 +38680,15 @@
       <c r="F61">
         <v>281.25</v>
       </c>
-      <c r="G61" t="str">
+      <c r="H61" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(60,1') = 281.25;</v>
+        <v>TX1(60,1) = 281.25;</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(61,0') = 0;</v>
+        <v>TX1(61,0) = 0;</v>
       </c>
       <c r="C62">
         <f t="shared" si="2"/>
@@ -38705,15 +38704,15 @@
       <c r="F62">
         <v>285.9375</v>
       </c>
-      <c r="G62" t="str">
+      <c r="H62" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(61,1') = 285.9375;</v>
+        <v>TX1(61,1) = 285.9375;</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(62,0') = 0;</v>
+        <v>TX1(62,0) = 0;</v>
       </c>
       <c r="C63">
         <f t="shared" si="2"/>
@@ -38729,15 +38728,15 @@
       <c r="F63">
         <v>290.625</v>
       </c>
-      <c r="G63" t="str">
+      <c r="H63" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(62,1') = 290.625;</v>
+        <v>TX1(62,1) = 290.625;</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(63,0') = 0;</v>
+        <v>TX1(63,0) = 0;</v>
       </c>
       <c r="C64">
         <f t="shared" si="2"/>
@@ -38753,15 +38752,15 @@
       <c r="F64">
         <v>295.3125</v>
       </c>
-      <c r="G64" t="str">
+      <c r="H64" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(63,1') = 295.3125;</v>
+        <v>TX1(63,1) = 295.3125;</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f t="shared" si="0"/>
-        <v>TX1(64,0') = 0;</v>
+        <v>TX1(64,0) = 0;</v>
       </c>
       <c r="C65">
         <f t="shared" si="2"/>
@@ -38777,15 +38776,15 @@
       <c r="F65">
         <v>300</v>
       </c>
-      <c r="G65" t="str">
+      <c r="H65" t="str">
         <f t="shared" si="1"/>
-        <v>TX1(64,1') = 300;</v>
+        <v>TX1(64,1) = 300;</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
-        <f t="shared" ref="B66:B129" si="4">_xlfn.CONCAT("TX1(",C66,",0","') = ",E66,";")</f>
-        <v>TX1(65,0') = 0.432499999999999;</v>
+        <f t="shared" ref="B66:B129" si="4">_xlfn.CONCAT("TX1(",C66,",0",") = ",E66,";")</f>
+        <v>TX1(65,0) = 0.432499999999999;</v>
       </c>
       <c r="C66">
         <f t="shared" si="2"/>
@@ -38801,15 +38800,15 @@
       <c r="F66">
         <v>0</v>
       </c>
-      <c r="G66" t="str">
-        <f t="shared" ref="G66:G129" si="5">_xlfn.CONCAT("TX1(",C66,",1","') = ",F66,";")</f>
-        <v>TX1(65,1') = 0;</v>
+      <c r="H66" t="str">
+        <f t="shared" ref="H66:H129" si="5">_xlfn.CONCAT("TX1(",C66,",1",") = ",F66,";")</f>
+        <v>TX1(65,1) = 0;</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(66,0') = 0.432499999999999;</v>
+        <v>TX1(66,0) = 0.432499999999999;</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C130" si="6">C66+1</f>
@@ -38825,15 +38824,15 @@
       <c r="F67">
         <v>4.6875</v>
       </c>
-      <c r="G67" t="str">
+      <c r="H67" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(66,1') = 4.6875;</v>
+        <v>TX1(66,1) = 4.6875;</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(67,0') = 0.432499999999999;</v>
+        <v>TX1(67,0) = 0.432499999999999;</v>
       </c>
       <c r="C68">
         <f t="shared" si="6"/>
@@ -38849,15 +38848,15 @@
       <c r="F68">
         <v>9.375</v>
       </c>
-      <c r="G68" t="str">
+      <c r="H68" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(67,1') = 9.375;</v>
+        <v>TX1(67,1) = 9.375;</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(68,0') = 0.432499999999999;</v>
+        <v>TX1(68,0) = 0.432499999999999;</v>
       </c>
       <c r="C69">
         <f t="shared" si="6"/>
@@ -38873,15 +38872,15 @@
       <c r="F69">
         <v>14.0625</v>
       </c>
-      <c r="G69" t="str">
+      <c r="H69" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(68,1') = 14.0625;</v>
+        <v>TX1(68,1) = 14.0625;</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(69,0') = 0.432499999999999;</v>
+        <v>TX1(69,0) = 0.432499999999999;</v>
       </c>
       <c r="C70">
         <f t="shared" si="6"/>
@@ -38897,15 +38896,15 @@
       <c r="F70">
         <v>18.75</v>
       </c>
-      <c r="G70" t="str">
+      <c r="H70" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(69,1') = 18.75;</v>
+        <v>TX1(69,1) = 18.75;</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(70,0') = 0.432499999999999;</v>
+        <v>TX1(70,0) = 0.432499999999999;</v>
       </c>
       <c r="C71">
         <f t="shared" si="6"/>
@@ -38921,15 +38920,15 @@
       <c r="F71">
         <v>23.4375</v>
       </c>
-      <c r="G71" t="str">
+      <c r="H71" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(70,1') = 23.4375;</v>
+        <v>TX1(70,1) = 23.4375;</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(71,0') = 0.432499999999999;</v>
+        <v>TX1(71,0) = 0.432499999999999;</v>
       </c>
       <c r="C72">
         <f t="shared" si="6"/>
@@ -38945,15 +38944,15 @@
       <c r="F72">
         <v>28.125</v>
       </c>
-      <c r="G72" t="str">
+      <c r="H72" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(71,1') = 28.125;</v>
+        <v>TX1(71,1) = 28.125;</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(72,0') = 0.432499999999999;</v>
+        <v>TX1(72,0) = 0.432499999999999;</v>
       </c>
       <c r="C73">
         <f t="shared" si="6"/>
@@ -38969,15 +38968,15 @@
       <c r="F73">
         <v>32.8125</v>
       </c>
-      <c r="G73" t="str">
+      <c r="H73" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(72,1') = 32.8125;</v>
+        <v>TX1(72,1) = 32.8125;</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(73,0') = 0.432499999999999;</v>
+        <v>TX1(73,0) = 0.432499999999999;</v>
       </c>
       <c r="C74">
         <f t="shared" si="6"/>
@@ -38993,15 +38992,15 @@
       <c r="F74">
         <v>37.5</v>
       </c>
-      <c r="G74" t="str">
+      <c r="H74" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(73,1') = 37.5;</v>
+        <v>TX1(73,1) = 37.5;</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(74,0') = 0.432499999999999;</v>
+        <v>TX1(74,0) = 0.432499999999999;</v>
       </c>
       <c r="C75">
         <f t="shared" si="6"/>
@@ -39017,15 +39016,15 @@
       <c r="F75">
         <v>42.1875</v>
       </c>
-      <c r="G75" t="str">
+      <c r="H75" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(74,1') = 42.1875;</v>
+        <v>TX1(74,1) = 42.1875;</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(75,0') = 0.432499999999999;</v>
+        <v>TX1(75,0) = 0.432499999999999;</v>
       </c>
       <c r="C76">
         <f t="shared" si="6"/>
@@ -39041,15 +39040,15 @@
       <c r="F76">
         <v>46.875</v>
       </c>
-      <c r="G76" t="str">
+      <c r="H76" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(75,1') = 46.875;</v>
+        <v>TX1(75,1) = 46.875;</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(76,0') = 0.432499999999999;</v>
+        <v>TX1(76,0) = 0.432499999999999;</v>
       </c>
       <c r="C77">
         <f t="shared" si="6"/>
@@ -39065,15 +39064,15 @@
       <c r="F77">
         <v>51.5625</v>
       </c>
-      <c r="G77" t="str">
+      <c r="H77" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(76,1') = 51.5625;</v>
+        <v>TX1(76,1) = 51.5625;</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(77,0') = 0.432499999999999;</v>
+        <v>TX1(77,0) = 0.432499999999999;</v>
       </c>
       <c r="C78">
         <f t="shared" si="6"/>
@@ -39089,15 +39088,15 @@
       <c r="F78">
         <v>56.25</v>
       </c>
-      <c r="G78" t="str">
+      <c r="H78" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(77,1') = 56.25;</v>
+        <v>TX1(77,1) = 56.25;</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(78,0') = 0.432499999999999;</v>
+        <v>TX1(78,0) = 0.432499999999999;</v>
       </c>
       <c r="C79">
         <f t="shared" si="6"/>
@@ -39113,15 +39112,15 @@
       <c r="F79">
         <v>60.9375</v>
       </c>
-      <c r="G79" t="str">
+      <c r="H79" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(78,1') = 60.9375;</v>
+        <v>TX1(78,1) = 60.9375;</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(79,0') = 0.432499999999999;</v>
+        <v>TX1(79,0) = 0.432499999999999;</v>
       </c>
       <c r="C80">
         <f t="shared" si="6"/>
@@ -39137,15 +39136,15 @@
       <c r="F80">
         <v>65.625</v>
       </c>
-      <c r="G80" t="str">
+      <c r="H80" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(79,1') = 65.625;</v>
+        <v>TX1(79,1) = 65.625;</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(80,0') = 0.432499999999999;</v>
+        <v>TX1(80,0) = 0.432499999999999;</v>
       </c>
       <c r="C81">
         <f t="shared" si="6"/>
@@ -39161,15 +39160,15 @@
       <c r="F81">
         <v>70.3125</v>
       </c>
-      <c r="G81" t="str">
+      <c r="H81" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(80,1') = 70.3125;</v>
+        <v>TX1(80,1) = 70.3125;</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(81,0') = 0.432499999999999;</v>
+        <v>TX1(81,0) = 0.432499999999999;</v>
       </c>
       <c r="C82">
         <f t="shared" si="6"/>
@@ -39185,15 +39184,15 @@
       <c r="F82">
         <v>75</v>
       </c>
-      <c r="G82" t="str">
+      <c r="H82" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(81,1') = 75;</v>
+        <v>TX1(81,1) = 75;</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(82,0') = 0.432499999999999;</v>
+        <v>TX1(82,0) = 0.432499999999999;</v>
       </c>
       <c r="C83">
         <f t="shared" si="6"/>
@@ -39209,15 +39208,15 @@
       <c r="F83">
         <v>79.6875</v>
       </c>
-      <c r="G83" t="str">
+      <c r="H83" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(82,1') = 79.6875;</v>
+        <v>TX1(82,1) = 79.6875;</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(83,0') = 0.432499999999999;</v>
+        <v>TX1(83,0) = 0.432499999999999;</v>
       </c>
       <c r="C84">
         <f t="shared" si="6"/>
@@ -39233,15 +39232,15 @@
       <c r="F84">
         <v>84.375</v>
       </c>
-      <c r="G84" t="str">
+      <c r="H84" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(83,1') = 84.375;</v>
+        <v>TX1(83,1) = 84.375;</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(84,0') = 0.432499999999999;</v>
+        <v>TX1(84,0) = 0.432499999999999;</v>
       </c>
       <c r="C85">
         <f t="shared" si="6"/>
@@ -39257,15 +39256,15 @@
       <c r="F85">
         <v>89.0625</v>
       </c>
-      <c r="G85" t="str">
+      <c r="H85" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(84,1') = 89.0625;</v>
+        <v>TX1(84,1) = 89.0625;</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(85,0') = 0.432499999999999;</v>
+        <v>TX1(85,0) = 0.432499999999999;</v>
       </c>
       <c r="C86">
         <f t="shared" si="6"/>
@@ -39281,15 +39280,15 @@
       <c r="F86">
         <v>93.75</v>
       </c>
-      <c r="G86" t="str">
+      <c r="H86" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(85,1') = 93.75;</v>
+        <v>TX1(85,1) = 93.75;</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(86,0') = 0.432499999999999;</v>
+        <v>TX1(86,0) = 0.432499999999999;</v>
       </c>
       <c r="C87">
         <f t="shared" si="6"/>
@@ -39305,15 +39304,15 @@
       <c r="F87">
         <v>98.4375</v>
       </c>
-      <c r="G87" t="str">
+      <c r="H87" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(86,1') = 98.4375;</v>
+        <v>TX1(86,1) = 98.4375;</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(87,0') = 0.432499999999999;</v>
+        <v>TX1(87,0) = 0.432499999999999;</v>
       </c>
       <c r="C88">
         <f t="shared" si="6"/>
@@ -39329,15 +39328,15 @@
       <c r="F88">
         <v>103.125</v>
       </c>
-      <c r="G88" t="str">
+      <c r="H88" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(87,1') = 103.125;</v>
+        <v>TX1(87,1) = 103.125;</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(88,0') = 0.432499999999999;</v>
+        <v>TX1(88,0) = 0.432499999999999;</v>
       </c>
       <c r="C89">
         <f t="shared" si="6"/>
@@ -39353,15 +39352,15 @@
       <c r="F89">
         <v>107.8125</v>
       </c>
-      <c r="G89" t="str">
+      <c r="H89" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(88,1') = 107.8125;</v>
+        <v>TX1(88,1) = 107.8125;</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(89,0') = 0.432499999999999;</v>
+        <v>TX1(89,0) = 0.432499999999999;</v>
       </c>
       <c r="C90">
         <f t="shared" si="6"/>
@@ -39377,15 +39376,15 @@
       <c r="F90">
         <v>112.5</v>
       </c>
-      <c r="G90" t="str">
+      <c r="H90" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(89,1') = 112.5;</v>
+        <v>TX1(89,1) = 112.5;</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(90,0') = 0.432499999999999;</v>
+        <v>TX1(90,0) = 0.432499999999999;</v>
       </c>
       <c r="C91">
         <f t="shared" si="6"/>
@@ -39401,15 +39400,15 @@
       <c r="F91">
         <v>117.1875</v>
       </c>
-      <c r="G91" t="str">
+      <c r="H91" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(90,1') = 117.1875;</v>
+        <v>TX1(90,1) = 117.1875;</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(91,0') = 0.432499999999999;</v>
+        <v>TX1(91,0) = 0.432499999999999;</v>
       </c>
       <c r="C92">
         <f t="shared" si="6"/>
@@ -39425,15 +39424,15 @@
       <c r="F92">
         <v>121.875</v>
       </c>
-      <c r="G92" t="str">
+      <c r="H92" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(91,1') = 121.875;</v>
+        <v>TX1(91,1) = 121.875;</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(92,0') = 0.432499999999999;</v>
+        <v>TX1(92,0) = 0.432499999999999;</v>
       </c>
       <c r="C93">
         <f t="shared" si="6"/>
@@ -39449,15 +39448,15 @@
       <c r="F93">
         <v>126.5625</v>
       </c>
-      <c r="G93" t="str">
+      <c r="H93" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(92,1') = 126.5625;</v>
+        <v>TX1(92,1) = 126.5625;</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(93,0') = 0.432499999999999;</v>
+        <v>TX1(93,0) = 0.432499999999999;</v>
       </c>
       <c r="C94">
         <f t="shared" si="6"/>
@@ -39473,15 +39472,15 @@
       <c r="F94">
         <v>131.25</v>
       </c>
-      <c r="G94" t="str">
+      <c r="H94" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(93,1') = 131.25;</v>
+        <v>TX1(93,1) = 131.25;</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(94,0') = 0.432499999999999;</v>
+        <v>TX1(94,0) = 0.432499999999999;</v>
       </c>
       <c r="C95">
         <f t="shared" si="6"/>
@@ -39497,15 +39496,15 @@
       <c r="F95">
         <v>135.9375</v>
       </c>
-      <c r="G95" t="str">
+      <c r="H95" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(94,1') = 135.9375;</v>
+        <v>TX1(94,1) = 135.9375;</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(95,0') = 0.432499999999999;</v>
+        <v>TX1(95,0) = 0.432499999999999;</v>
       </c>
       <c r="C96">
         <f t="shared" si="6"/>
@@ -39521,15 +39520,15 @@
       <c r="F96">
         <v>140.625</v>
       </c>
-      <c r="G96" t="str">
+      <c r="H96" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(95,1') = 140.625;</v>
+        <v>TX1(95,1) = 140.625;</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(96,0') = 0.432499999999999;</v>
+        <v>TX1(96,0) = 0.432499999999999;</v>
       </c>
       <c r="C97">
         <f t="shared" si="6"/>
@@ -39545,15 +39544,15 @@
       <c r="F97">
         <v>145.3125</v>
       </c>
-      <c r="G97" t="str">
+      <c r="H97" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(96,1') = 145.3125;</v>
+        <v>TX1(96,1) = 145.3125;</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(97,0') = 0.432499999999999;</v>
+        <v>TX1(97,0) = 0.432499999999999;</v>
       </c>
       <c r="C98">
         <f t="shared" si="6"/>
@@ -39569,15 +39568,15 @@
       <c r="F98">
         <v>150</v>
       </c>
-      <c r="G98" t="str">
+      <c r="H98" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(97,1') = 150;</v>
+        <v>TX1(97,1) = 150;</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(98,0') = 0.432499999999999;</v>
+        <v>TX1(98,0) = 0.432499999999999;</v>
       </c>
       <c r="C99">
         <f t="shared" si="6"/>
@@ -39593,15 +39592,15 @@
       <c r="F99">
         <v>154.6875</v>
       </c>
-      <c r="G99" t="str">
+      <c r="H99" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(98,1') = 154.6875;</v>
+        <v>TX1(98,1) = 154.6875;</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(99,0') = 0.432499999999999;</v>
+        <v>TX1(99,0) = 0.432499999999999;</v>
       </c>
       <c r="C100">
         <f t="shared" si="6"/>
@@ -39617,15 +39616,15 @@
       <c r="F100">
         <v>159.375</v>
       </c>
-      <c r="G100" t="str">
+      <c r="H100" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(99,1') = 159.375;</v>
+        <v>TX1(99,1) = 159.375;</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(100,0') = 0.432499999999999;</v>
+        <v>TX1(100,0) = 0.432499999999999;</v>
       </c>
       <c r="C101">
         <f t="shared" si="6"/>
@@ -39641,15 +39640,15 @@
       <c r="F101">
         <v>164.0625</v>
       </c>
-      <c r="G101" t="str">
+      <c r="H101" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(100,1') = 164.0625;</v>
+        <v>TX1(100,1) = 164.0625;</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(101,0') = 0.432499999999999;</v>
+        <v>TX1(101,0) = 0.432499999999999;</v>
       </c>
       <c r="C102">
         <f t="shared" si="6"/>
@@ -39665,15 +39664,15 @@
       <c r="F102">
         <v>168.75</v>
       </c>
-      <c r="G102" t="str">
+      <c r="H102" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(101,1') = 168.75;</v>
+        <v>TX1(101,1) = 168.75;</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(102,0') = 0.432499999999999;</v>
+        <v>TX1(102,0) = 0.432499999999999;</v>
       </c>
       <c r="C103">
         <f t="shared" si="6"/>
@@ -39689,15 +39688,15 @@
       <c r="F103">
         <v>173.4375</v>
       </c>
-      <c r="G103" t="str">
+      <c r="H103" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(102,1') = 173.4375;</v>
+        <v>TX1(102,1) = 173.4375;</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(103,0') = 0.432499999999999;</v>
+        <v>TX1(103,0) = 0.432499999999999;</v>
       </c>
       <c r="C104">
         <f t="shared" si="6"/>
@@ -39713,15 +39712,15 @@
       <c r="F104">
         <v>178.125</v>
       </c>
-      <c r="G104" t="str">
+      <c r="H104" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(103,1') = 178.125;</v>
+        <v>TX1(103,1) = 178.125;</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(104,0') = 0.432499999999999;</v>
+        <v>TX1(104,0) = 0.432499999999999;</v>
       </c>
       <c r="C105">
         <f t="shared" si="6"/>
@@ -39737,15 +39736,15 @@
       <c r="F105">
         <v>182.8125</v>
       </c>
-      <c r="G105" t="str">
+      <c r="H105" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(104,1') = 182.8125;</v>
+        <v>TX1(104,1) = 182.8125;</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(105,0') = 0.432499999999999;</v>
+        <v>TX1(105,0) = 0.432499999999999;</v>
       </c>
       <c r="C106">
         <f t="shared" si="6"/>
@@ -39761,15 +39760,15 @@
       <c r="F106">
         <v>187.5</v>
       </c>
-      <c r="G106" t="str">
+      <c r="H106" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(105,1') = 187.5;</v>
+        <v>TX1(105,1) = 187.5;</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(106,0') = 0.432499999999999;</v>
+        <v>TX1(106,0) = 0.432499999999999;</v>
       </c>
       <c r="C107">
         <f t="shared" si="6"/>
@@ -39785,15 +39784,15 @@
       <c r="F107">
         <v>192.1875</v>
       </c>
-      <c r="G107" t="str">
+      <c r="H107" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(106,1') = 192.1875;</v>
+        <v>TX1(106,1) = 192.1875;</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(107,0') = 0.432499999999999;</v>
+        <v>TX1(107,0) = 0.432499999999999;</v>
       </c>
       <c r="C108">
         <f t="shared" si="6"/>
@@ -39809,15 +39808,15 @@
       <c r="F108">
         <v>196.875</v>
       </c>
-      <c r="G108" t="str">
+      <c r="H108" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(107,1') = 196.875;</v>
+        <v>TX1(107,1) = 196.875;</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(108,0') = 0.432499999999999;</v>
+        <v>TX1(108,0) = 0.432499999999999;</v>
       </c>
       <c r="C109">
         <f t="shared" si="6"/>
@@ -39833,15 +39832,15 @@
       <c r="F109">
         <v>201.5625</v>
       </c>
-      <c r="G109" t="str">
+      <c r="H109" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(108,1') = 201.5625;</v>
+        <v>TX1(108,1) = 201.5625;</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(109,0') = 0.432499999999999;</v>
+        <v>TX1(109,0) = 0.432499999999999;</v>
       </c>
       <c r="C110">
         <f t="shared" si="6"/>
@@ -39857,15 +39856,15 @@
       <c r="F110">
         <v>206.25</v>
       </c>
-      <c r="G110" t="str">
+      <c r="H110" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(109,1') = 206.25;</v>
+        <v>TX1(109,1) = 206.25;</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(110,0') = 0.432499999999999;</v>
+        <v>TX1(110,0) = 0.432499999999999;</v>
       </c>
       <c r="C111">
         <f t="shared" si="6"/>
@@ -39881,15 +39880,15 @@
       <c r="F111">
         <v>210.9375</v>
       </c>
-      <c r="G111" t="str">
+      <c r="H111" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(110,1') = 210.9375;</v>
+        <v>TX1(110,1) = 210.9375;</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(111,0') = 0.432499999999999;</v>
+        <v>TX1(111,0) = 0.432499999999999;</v>
       </c>
       <c r="C112">
         <f t="shared" si="6"/>
@@ -39905,15 +39904,15 @@
       <c r="F112">
         <v>215.625</v>
       </c>
-      <c r="G112" t="str">
+      <c r="H112" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(111,1') = 215.625;</v>
+        <v>TX1(111,1) = 215.625;</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(112,0') = 0.432499999999999;</v>
+        <v>TX1(112,0) = 0.432499999999999;</v>
       </c>
       <c r="C113">
         <f t="shared" si="6"/>
@@ -39929,15 +39928,15 @@
       <c r="F113">
         <v>220.3125</v>
       </c>
-      <c r="G113" t="str">
+      <c r="H113" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(112,1') = 220.3125;</v>
+        <v>TX1(112,1) = 220.3125;</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(113,0') = 0.432499999999999;</v>
+        <v>TX1(113,0) = 0.432499999999999;</v>
       </c>
       <c r="C114">
         <f t="shared" si="6"/>
@@ -39953,15 +39952,15 @@
       <c r="F114">
         <v>225</v>
       </c>
-      <c r="G114" t="str">
+      <c r="H114" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(113,1') = 225;</v>
+        <v>TX1(113,1) = 225;</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(114,0') = 0.432499999999999;</v>
+        <v>TX1(114,0) = 0.432499999999999;</v>
       </c>
       <c r="C115">
         <f t="shared" si="6"/>
@@ -39977,15 +39976,15 @@
       <c r="F115">
         <v>229.6875</v>
       </c>
-      <c r="G115" t="str">
+      <c r="H115" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(114,1') = 229.6875;</v>
+        <v>TX1(114,1) = 229.6875;</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(115,0') = 0.432499999999999;</v>
+        <v>TX1(115,0) = 0.432499999999999;</v>
       </c>
       <c r="C116">
         <f t="shared" si="6"/>
@@ -40001,15 +40000,15 @@
       <c r="F116">
         <v>234.375</v>
       </c>
-      <c r="G116" t="str">
+      <c r="H116" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(115,1') = 234.375;</v>
+        <v>TX1(115,1) = 234.375;</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(116,0') = 0.432499999999999;</v>
+        <v>TX1(116,0) = 0.432499999999999;</v>
       </c>
       <c r="C117">
         <f t="shared" si="6"/>
@@ -40025,15 +40024,15 @@
       <c r="F117">
         <v>239.0625</v>
       </c>
-      <c r="G117" t="str">
+      <c r="H117" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(116,1') = 239.0625;</v>
+        <v>TX1(116,1) = 239.0625;</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(117,0') = 0.432499999999999;</v>
+        <v>TX1(117,0) = 0.432499999999999;</v>
       </c>
       <c r="C118">
         <f t="shared" si="6"/>
@@ -40049,15 +40048,15 @@
       <c r="F118">
         <v>243.75</v>
       </c>
-      <c r="G118" t="str">
+      <c r="H118" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(117,1') = 243.75;</v>
+        <v>TX1(117,1) = 243.75;</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(118,0') = 0.432499999999999;</v>
+        <v>TX1(118,0) = 0.432499999999999;</v>
       </c>
       <c r="C119">
         <f t="shared" si="6"/>
@@ -40073,15 +40072,15 @@
       <c r="F119">
         <v>248.4375</v>
       </c>
-      <c r="G119" t="str">
+      <c r="H119" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(118,1') = 248.4375;</v>
+        <v>TX1(118,1) = 248.4375;</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(119,0') = 0.432499999999999;</v>
+        <v>TX1(119,0) = 0.432499999999999;</v>
       </c>
       <c r="C120">
         <f t="shared" si="6"/>
@@ -40097,15 +40096,15 @@
       <c r="F120">
         <v>253.125</v>
       </c>
-      <c r="G120" t="str">
+      <c r="H120" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(119,1') = 253.125;</v>
+        <v>TX1(119,1) = 253.125;</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(120,0') = 0.432499999999999;</v>
+        <v>TX1(120,0) = 0.432499999999999;</v>
       </c>
       <c r="C121">
         <f t="shared" si="6"/>
@@ -40121,15 +40120,15 @@
       <c r="F121">
         <v>257.8125</v>
       </c>
-      <c r="G121" t="str">
+      <c r="H121" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(120,1') = 257.8125;</v>
+        <v>TX1(120,1) = 257.8125;</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(121,0') = 0.432499999999999;</v>
+        <v>TX1(121,0) = 0.432499999999999;</v>
       </c>
       <c r="C122">
         <f t="shared" si="6"/>
@@ -40145,15 +40144,15 @@
       <c r="F122">
         <v>262.5</v>
       </c>
-      <c r="G122" t="str">
+      <c r="H122" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(121,1') = 262.5;</v>
+        <v>TX1(121,1) = 262.5;</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(122,0') = 0.432499999999999;</v>
+        <v>TX1(122,0) = 0.432499999999999;</v>
       </c>
       <c r="C123">
         <f t="shared" si="6"/>
@@ -40169,15 +40168,15 @@
       <c r="F123">
         <v>267.1875</v>
       </c>
-      <c r="G123" t="str">
+      <c r="H123" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(122,1') = 267.1875;</v>
+        <v>TX1(122,1) = 267.1875;</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(123,0') = 0.432499999999999;</v>
+        <v>TX1(123,0) = 0.432499999999999;</v>
       </c>
       <c r="C124">
         <f t="shared" si="6"/>
@@ -40193,15 +40192,15 @@
       <c r="F124">
         <v>271.875</v>
       </c>
-      <c r="G124" t="str">
+      <c r="H124" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(123,1') = 271.875;</v>
+        <v>TX1(123,1) = 271.875;</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(124,0') = 0.432499999999999;</v>
+        <v>TX1(124,0) = 0.432499999999999;</v>
       </c>
       <c r="C125">
         <f t="shared" si="6"/>
@@ -40217,15 +40216,15 @@
       <c r="F125">
         <v>276.5625</v>
       </c>
-      <c r="G125" t="str">
+      <c r="H125" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(124,1') = 276.5625;</v>
+        <v>TX1(124,1) = 276.5625;</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(125,0') = 0.432499999999999;</v>
+        <v>TX1(125,0) = 0.432499999999999;</v>
       </c>
       <c r="C126">
         <f t="shared" si="6"/>
@@ -40241,15 +40240,15 @@
       <c r="F126">
         <v>281.25</v>
       </c>
-      <c r="G126" t="str">
+      <c r="H126" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(125,1') = 281.25;</v>
+        <v>TX1(125,1) = 281.25;</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(126,0') = 0.432499999999999;</v>
+        <v>TX1(126,0) = 0.432499999999999;</v>
       </c>
       <c r="C127">
         <f t="shared" si="6"/>
@@ -40265,15 +40264,15 @@
       <c r="F127">
         <v>285.9375</v>
       </c>
-      <c r="G127" t="str">
+      <c r="H127" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(126,1') = 285.9375;</v>
+        <v>TX1(126,1) = 285.9375;</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(127,0') = 0.432499999999999;</v>
+        <v>TX1(127,0) = 0.432499999999999;</v>
       </c>
       <c r="C128">
         <f t="shared" si="6"/>
@@ -40289,15 +40288,15 @@
       <c r="F128">
         <v>290.625</v>
       </c>
-      <c r="G128" t="str">
+      <c r="H128" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(127,1') = 290.625;</v>
+        <v>TX1(127,1) = 290.625;</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" t="str">
         <f t="shared" si="4"/>
-        <v>TX1(128,0') = 0.432499999999999;</v>
+        <v>TX1(128,0) = 0.432499999999999;</v>
       </c>
       <c r="C129">
         <f t="shared" si="6"/>
@@ -40313,15 +40312,15 @@
       <c r="F129">
         <v>295.3125</v>
       </c>
-      <c r="G129" t="str">
+      <c r="H129" t="str">
         <f t="shared" si="5"/>
-        <v>TX1(128,1') = 295.3125;</v>
+        <v>TX1(128,1) = 295.3125;</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" t="str">
-        <f t="shared" ref="B130:B193" si="8">_xlfn.CONCAT("TX1(",C130,",0","') = ",E130,";")</f>
-        <v>TX1(129,0') = 0.432499999999999;</v>
+        <f t="shared" ref="B130:B193" si="8">_xlfn.CONCAT("TX1(",C130,",0",") = ",E130,";")</f>
+        <v>TX1(129,0) = 0.432499999999999;</v>
       </c>
       <c r="C130">
         <f t="shared" si="6"/>
@@ -40337,15 +40336,15 @@
       <c r="F130">
         <v>300</v>
       </c>
-      <c r="G130" t="str">
-        <f t="shared" ref="G130:G193" si="9">_xlfn.CONCAT("TX1(",C130,",1","') = ",F130,";")</f>
-        <v>TX1(129,1') = 300;</v>
+      <c r="H130" t="str">
+        <f t="shared" ref="H130:H193" si="9">_xlfn.CONCAT("TX1(",C130,",1",") = ",F130,";")</f>
+        <v>TX1(129,1) = 300;</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(130,0') = 0.864999999999999;</v>
+        <v>TX1(130,0) = 0.864999999999999;</v>
       </c>
       <c r="C131">
         <f t="shared" ref="C131:C194" si="10">C130+1</f>
@@ -40361,15 +40360,15 @@
       <c r="F131">
         <v>0</v>
       </c>
-      <c r="G131" t="str">
+      <c r="H131" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(130,1') = 0;</v>
+        <v>TX1(130,1) = 0;</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(131,0') = 0.864999999999999;</v>
+        <v>TX1(131,0) = 0.864999999999999;</v>
       </c>
       <c r="C132">
         <f t="shared" si="10"/>
@@ -40385,15 +40384,15 @@
       <c r="F132">
         <v>4.6875</v>
       </c>
-      <c r="G132" t="str">
+      <c r="H132" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(131,1') = 4.6875;</v>
+        <v>TX1(131,1) = 4.6875;</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(132,0') = 0.864999999999999;</v>
+        <v>TX1(132,0) = 0.864999999999999;</v>
       </c>
       <c r="C133">
         <f t="shared" si="10"/>
@@ -40409,15 +40408,15 @@
       <c r="F133">
         <v>9.375</v>
       </c>
-      <c r="G133" t="str">
+      <c r="H133" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(132,1') = 9.375;</v>
+        <v>TX1(132,1) = 9.375;</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(133,0') = 0.864999999999999;</v>
+        <v>TX1(133,0) = 0.864999999999999;</v>
       </c>
       <c r="C134">
         <f t="shared" si="10"/>
@@ -40433,15 +40432,15 @@
       <c r="F134">
         <v>14.0625</v>
       </c>
-      <c r="G134" t="str">
+      <c r="H134" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(133,1') = 14.0625;</v>
+        <v>TX1(133,1) = 14.0625;</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(134,0') = 0.864999999999999;</v>
+        <v>TX1(134,0) = 0.864999999999999;</v>
       </c>
       <c r="C135">
         <f t="shared" si="10"/>
@@ -40457,15 +40456,15 @@
       <c r="F135">
         <v>18.75</v>
       </c>
-      <c r="G135" t="str">
+      <c r="H135" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(134,1') = 18.75;</v>
+        <v>TX1(134,1) = 18.75;</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(135,0') = 0.864999999999999;</v>
+        <v>TX1(135,0) = 0.864999999999999;</v>
       </c>
       <c r="C136">
         <f t="shared" si="10"/>
@@ -40481,15 +40480,15 @@
       <c r="F136">
         <v>23.4375</v>
       </c>
-      <c r="G136" t="str">
+      <c r="H136" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(135,1') = 23.4375;</v>
+        <v>TX1(135,1) = 23.4375;</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(136,0') = 0.864999999999999;</v>
+        <v>TX1(136,0) = 0.864999999999999;</v>
       </c>
       <c r="C137">
         <f t="shared" si="10"/>
@@ -40505,15 +40504,15 @@
       <c r="F137">
         <v>28.125</v>
       </c>
-      <c r="G137" t="str">
+      <c r="H137" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(136,1') = 28.125;</v>
+        <v>TX1(136,1) = 28.125;</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(137,0') = 0.864999999999999;</v>
+        <v>TX1(137,0) = 0.864999999999999;</v>
       </c>
       <c r="C138">
         <f t="shared" si="10"/>
@@ -40529,15 +40528,15 @@
       <c r="F138">
         <v>32.8125</v>
       </c>
-      <c r="G138" t="str">
+      <c r="H138" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(137,1') = 32.8125;</v>
+        <v>TX1(137,1) = 32.8125;</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(138,0') = 0.864999999999999;</v>
+        <v>TX1(138,0) = 0.864999999999999;</v>
       </c>
       <c r="C139">
         <f t="shared" si="10"/>
@@ -40553,15 +40552,15 @@
       <c r="F139">
         <v>37.5</v>
       </c>
-      <c r="G139" t="str">
+      <c r="H139" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(138,1') = 37.5;</v>
+        <v>TX1(138,1) = 37.5;</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B140" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(139,0') = 0.864999999999999;</v>
+        <v>TX1(139,0) = 0.864999999999999;</v>
       </c>
       <c r="C140">
         <f t="shared" si="10"/>
@@ -40577,15 +40576,15 @@
       <c r="F140">
         <v>42.1875</v>
       </c>
-      <c r="G140" t="str">
+      <c r="H140" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(139,1') = 42.1875;</v>
+        <v>TX1(139,1) = 42.1875;</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(140,0') = 0.864999999999999;</v>
+        <v>TX1(140,0) = 0.864999999999999;</v>
       </c>
       <c r="C141">
         <f t="shared" si="10"/>
@@ -40601,15 +40600,15 @@
       <c r="F141">
         <v>46.875</v>
       </c>
-      <c r="G141" t="str">
+      <c r="H141" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(140,1') = 46.875;</v>
+        <v>TX1(140,1) = 46.875;</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(141,0') = 0.864999999999999;</v>
+        <v>TX1(141,0) = 0.864999999999999;</v>
       </c>
       <c r="C142">
         <f t="shared" si="10"/>
@@ -40625,15 +40624,15 @@
       <c r="F142">
         <v>51.5625</v>
       </c>
-      <c r="G142" t="str">
+      <c r="H142" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(141,1') = 51.5625;</v>
+        <v>TX1(141,1) = 51.5625;</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(142,0') = 0.864999999999999;</v>
+        <v>TX1(142,0) = 0.864999999999999;</v>
       </c>
       <c r="C143">
         <f t="shared" si="10"/>
@@ -40649,15 +40648,15 @@
       <c r="F143">
         <v>56.25</v>
       </c>
-      <c r="G143" t="str">
+      <c r="H143" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(142,1') = 56.25;</v>
+        <v>TX1(142,1) = 56.25;</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(143,0') = 0.864999999999999;</v>
+        <v>TX1(143,0) = 0.864999999999999;</v>
       </c>
       <c r="C144">
         <f t="shared" si="10"/>
@@ -40673,15 +40672,15 @@
       <c r="F144">
         <v>60.9375</v>
       </c>
-      <c r="G144" t="str">
+      <c r="H144" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(143,1') = 60.9375;</v>
+        <v>TX1(143,1) = 60.9375;</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(144,0') = 0.864999999999999;</v>
+        <v>TX1(144,0) = 0.864999999999999;</v>
       </c>
       <c r="C145">
         <f t="shared" si="10"/>
@@ -40697,15 +40696,15 @@
       <c r="F145">
         <v>65.625</v>
       </c>
-      <c r="G145" t="str">
+      <c r="H145" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(144,1') = 65.625;</v>
+        <v>TX1(144,1) = 65.625;</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(145,0') = 0.864999999999999;</v>
+        <v>TX1(145,0) = 0.864999999999999;</v>
       </c>
       <c r="C146">
         <f t="shared" si="10"/>
@@ -40721,15 +40720,15 @@
       <c r="F146">
         <v>70.3125</v>
       </c>
-      <c r="G146" t="str">
+      <c r="H146" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(145,1') = 70.3125;</v>
+        <v>TX1(145,1) = 70.3125;</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(146,0') = 0.864999999999999;</v>
+        <v>TX1(146,0) = 0.864999999999999;</v>
       </c>
       <c r="C147">
         <f t="shared" si="10"/>
@@ -40745,15 +40744,15 @@
       <c r="F147">
         <v>75</v>
       </c>
-      <c r="G147" t="str">
+      <c r="H147" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(146,1') = 75;</v>
+        <v>TX1(146,1) = 75;</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(147,0') = 0.864999999999999;</v>
+        <v>TX1(147,0) = 0.864999999999999;</v>
       </c>
       <c r="C148">
         <f t="shared" si="10"/>
@@ -40769,15 +40768,15 @@
       <c r="F148">
         <v>79.6875</v>
       </c>
-      <c r="G148" t="str">
+      <c r="H148" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(147,1') = 79.6875;</v>
+        <v>TX1(147,1) = 79.6875;</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(148,0') = 0.864999999999999;</v>
+        <v>TX1(148,0) = 0.864999999999999;</v>
       </c>
       <c r="C149">
         <f t="shared" si="10"/>
@@ -40793,15 +40792,15 @@
       <c r="F149">
         <v>84.375</v>
       </c>
-      <c r="G149" t="str">
+      <c r="H149" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(148,1') = 84.375;</v>
+        <v>TX1(148,1) = 84.375;</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(149,0') = 0.864999999999999;</v>
+        <v>TX1(149,0) = 0.864999999999999;</v>
       </c>
       <c r="C150">
         <f t="shared" si="10"/>
@@ -40817,15 +40816,15 @@
       <c r="F150">
         <v>89.0625</v>
       </c>
-      <c r="G150" t="str">
+      <c r="H150" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(149,1') = 89.0625;</v>
+        <v>TX1(149,1) = 89.0625;</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(150,0') = 0.864999999999999;</v>
+        <v>TX1(150,0) = 0.864999999999999;</v>
       </c>
       <c r="C151">
         <f t="shared" si="10"/>
@@ -40841,15 +40840,15 @@
       <c r="F151">
         <v>93.75</v>
       </c>
-      <c r="G151" t="str">
+      <c r="H151" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(150,1') = 93.75;</v>
+        <v>TX1(150,1) = 93.75;</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(151,0') = 0.864999999999999;</v>
+        <v>TX1(151,0) = 0.864999999999999;</v>
       </c>
       <c r="C152">
         <f t="shared" si="10"/>
@@ -40865,15 +40864,15 @@
       <c r="F152">
         <v>98.4375</v>
       </c>
-      <c r="G152" t="str">
+      <c r="H152" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(151,1') = 98.4375;</v>
+        <v>TX1(151,1) = 98.4375;</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(152,0') = 0.864999999999999;</v>
+        <v>TX1(152,0) = 0.864999999999999;</v>
       </c>
       <c r="C153">
         <f t="shared" si="10"/>
@@ -40889,15 +40888,15 @@
       <c r="F153">
         <v>103.125</v>
       </c>
-      <c r="G153" t="str">
+      <c r="H153" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(152,1') = 103.125;</v>
+        <v>TX1(152,1) = 103.125;</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(153,0') = 0.864999999999999;</v>
+        <v>TX1(153,0) = 0.864999999999999;</v>
       </c>
       <c r="C154">
         <f t="shared" si="10"/>
@@ -40913,15 +40912,15 @@
       <c r="F154">
         <v>107.8125</v>
       </c>
-      <c r="G154" t="str">
+      <c r="H154" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(153,1') = 107.8125;</v>
+        <v>TX1(153,1) = 107.8125;</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(154,0') = 0.864999999999999;</v>
+        <v>TX1(154,0) = 0.864999999999999;</v>
       </c>
       <c r="C155">
         <f t="shared" si="10"/>
@@ -40937,15 +40936,15 @@
       <c r="F155">
         <v>112.5</v>
       </c>
-      <c r="G155" t="str">
+      <c r="H155" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(154,1') = 112.5;</v>
+        <v>TX1(154,1) = 112.5;</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B156" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(155,0') = 0.864999999999999;</v>
+        <v>TX1(155,0) = 0.864999999999999;</v>
       </c>
       <c r="C156">
         <f t="shared" si="10"/>
@@ -40961,15 +40960,15 @@
       <c r="F156">
         <v>117.1875</v>
       </c>
-      <c r="G156" t="str">
+      <c r="H156" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(155,1') = 117.1875;</v>
+        <v>TX1(155,1) = 117.1875;</v>
       </c>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(156,0') = 0.864999999999999;</v>
+        <v>TX1(156,0) = 0.864999999999999;</v>
       </c>
       <c r="C157">
         <f t="shared" si="10"/>
@@ -40985,15 +40984,15 @@
       <c r="F157">
         <v>121.875</v>
       </c>
-      <c r="G157" t="str">
+      <c r="H157" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(156,1') = 121.875;</v>
+        <v>TX1(156,1) = 121.875;</v>
       </c>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(157,0') = 0.864999999999999;</v>
+        <v>TX1(157,0) = 0.864999999999999;</v>
       </c>
       <c r="C158">
         <f t="shared" si="10"/>
@@ -41009,15 +41008,15 @@
       <c r="F158">
         <v>126.5625</v>
       </c>
-      <c r="G158" t="str">
+      <c r="H158" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(157,1') = 126.5625;</v>
+        <v>TX1(157,1) = 126.5625;</v>
       </c>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(158,0') = 0.864999999999999;</v>
+        <v>TX1(158,0) = 0.864999999999999;</v>
       </c>
       <c r="C159">
         <f t="shared" si="10"/>
@@ -41033,15 +41032,15 @@
       <c r="F159">
         <v>131.25</v>
       </c>
-      <c r="G159" t="str">
+      <c r="H159" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(158,1') = 131.25;</v>
+        <v>TX1(158,1) = 131.25;</v>
       </c>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B160" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(159,0') = 0.864999999999999;</v>
+        <v>TX1(159,0) = 0.864999999999999;</v>
       </c>
       <c r="C160">
         <f t="shared" si="10"/>
@@ -41057,15 +41056,15 @@
       <c r="F160">
         <v>135.9375</v>
       </c>
-      <c r="G160" t="str">
+      <c r="H160" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(159,1') = 135.9375;</v>
+        <v>TX1(159,1) = 135.9375;</v>
       </c>
     </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B161" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(160,0') = 0.864999999999999;</v>
+        <v>TX1(160,0) = 0.864999999999999;</v>
       </c>
       <c r="C161">
         <f t="shared" si="10"/>
@@ -41081,15 +41080,15 @@
       <c r="F161">
         <v>140.625</v>
       </c>
-      <c r="G161" t="str">
+      <c r="H161" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(160,1') = 140.625;</v>
+        <v>TX1(160,1) = 140.625;</v>
       </c>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B162" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(161,0') = 0.864999999999999;</v>
+        <v>TX1(161,0) = 0.864999999999999;</v>
       </c>
       <c r="C162">
         <f t="shared" si="10"/>
@@ -41105,15 +41104,15 @@
       <c r="F162">
         <v>145.3125</v>
       </c>
-      <c r="G162" t="str">
+      <c r="H162" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(161,1') = 145.3125;</v>
+        <v>TX1(161,1) = 145.3125;</v>
       </c>
     </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B163" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(162,0') = 0.864999999999999;</v>
+        <v>TX1(162,0) = 0.864999999999999;</v>
       </c>
       <c r="C163">
         <f t="shared" si="10"/>
@@ -41129,15 +41128,15 @@
       <c r="F163">
         <v>150</v>
       </c>
-      <c r="G163" t="str">
+      <c r="H163" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(162,1') = 150;</v>
+        <v>TX1(162,1) = 150;</v>
       </c>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B164" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(163,0') = 0.864999999999999;</v>
+        <v>TX1(163,0) = 0.864999999999999;</v>
       </c>
       <c r="C164">
         <f t="shared" si="10"/>
@@ -41153,15 +41152,15 @@
       <c r="F164">
         <v>154.6875</v>
       </c>
-      <c r="G164" t="str">
+      <c r="H164" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(163,1') = 154.6875;</v>
+        <v>TX1(163,1) = 154.6875;</v>
       </c>
     </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(164,0') = 0.864999999999999;</v>
+        <v>TX1(164,0) = 0.864999999999999;</v>
       </c>
       <c r="C165">
         <f t="shared" si="10"/>
@@ -41177,15 +41176,15 @@
       <c r="F165">
         <v>159.375</v>
       </c>
-      <c r="G165" t="str">
+      <c r="H165" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(164,1') = 159.375;</v>
+        <v>TX1(164,1) = 159.375;</v>
       </c>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(165,0') = 0.864999999999999;</v>
+        <v>TX1(165,0) = 0.864999999999999;</v>
       </c>
       <c r="C166">
         <f t="shared" si="10"/>
@@ -41201,15 +41200,15 @@
       <c r="F166">
         <v>164.0625</v>
       </c>
-      <c r="G166" t="str">
+      <c r="H166" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(165,1') = 164.0625;</v>
+        <v>TX1(165,1) = 164.0625;</v>
       </c>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B167" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(166,0') = 0.864999999999999;</v>
+        <v>TX1(166,0) = 0.864999999999999;</v>
       </c>
       <c r="C167">
         <f t="shared" si="10"/>
@@ -41225,15 +41224,15 @@
       <c r="F167">
         <v>168.75</v>
       </c>
-      <c r="G167" t="str">
+      <c r="H167" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(166,1') = 168.75;</v>
+        <v>TX1(166,1) = 168.75;</v>
       </c>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B168" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(167,0') = 0.864999999999999;</v>
+        <v>TX1(167,0) = 0.864999999999999;</v>
       </c>
       <c r="C168">
         <f t="shared" si="10"/>
@@ -41249,15 +41248,15 @@
       <c r="F168">
         <v>173.4375</v>
       </c>
-      <c r="G168" t="str">
+      <c r="H168" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(167,1') = 173.4375;</v>
+        <v>TX1(167,1) = 173.4375;</v>
       </c>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B169" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(168,0') = 0.864999999999999;</v>
+        <v>TX1(168,0) = 0.864999999999999;</v>
       </c>
       <c r="C169">
         <f t="shared" si="10"/>
@@ -41273,15 +41272,15 @@
       <c r="F169">
         <v>178.125</v>
       </c>
-      <c r="G169" t="str">
+      <c r="H169" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(168,1') = 178.125;</v>
+        <v>TX1(168,1) = 178.125;</v>
       </c>
     </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(169,0') = 0.864999999999999;</v>
+        <v>TX1(169,0) = 0.864999999999999;</v>
       </c>
       <c r="C170">
         <f t="shared" si="10"/>
@@ -41297,15 +41296,15 @@
       <c r="F170">
         <v>182.8125</v>
       </c>
-      <c r="G170" t="str">
+      <c r="H170" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(169,1') = 182.8125;</v>
+        <v>TX1(169,1) = 182.8125;</v>
       </c>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(170,0') = 0.864999999999999;</v>
+        <v>TX1(170,0) = 0.864999999999999;</v>
       </c>
       <c r="C171">
         <f t="shared" si="10"/>
@@ -41321,15 +41320,15 @@
       <c r="F171">
         <v>187.5</v>
       </c>
-      <c r="G171" t="str">
+      <c r="H171" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(170,1') = 187.5;</v>
+        <v>TX1(170,1) = 187.5;</v>
       </c>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(171,0') = 0.864999999999999;</v>
+        <v>TX1(171,0) = 0.864999999999999;</v>
       </c>
       <c r="C172">
         <f t="shared" si="10"/>
@@ -41345,15 +41344,15 @@
       <c r="F172">
         <v>192.1875</v>
       </c>
-      <c r="G172" t="str">
+      <c r="H172" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(171,1') = 192.1875;</v>
+        <v>TX1(171,1) = 192.1875;</v>
       </c>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B173" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(172,0') = 0.864999999999999;</v>
+        <v>TX1(172,0) = 0.864999999999999;</v>
       </c>
       <c r="C173">
         <f t="shared" si="10"/>
@@ -41369,15 +41368,15 @@
       <c r="F173">
         <v>196.875</v>
       </c>
-      <c r="G173" t="str">
+      <c r="H173" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(172,1') = 196.875;</v>
+        <v>TX1(172,1) = 196.875;</v>
       </c>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B174" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(173,0') = 0.864999999999999;</v>
+        <v>TX1(173,0) = 0.864999999999999;</v>
       </c>
       <c r="C174">
         <f t="shared" si="10"/>
@@ -41393,15 +41392,15 @@
       <c r="F174">
         <v>201.5625</v>
       </c>
-      <c r="G174" t="str">
+      <c r="H174" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(173,1') = 201.5625;</v>
+        <v>TX1(173,1) = 201.5625;</v>
       </c>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B175" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(174,0') = 0.864999999999999;</v>
+        <v>TX1(174,0) = 0.864999999999999;</v>
       </c>
       <c r="C175">
         <f t="shared" si="10"/>
@@ -41417,15 +41416,15 @@
       <c r="F175">
         <v>206.25</v>
       </c>
-      <c r="G175" t="str">
+      <c r="H175" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(174,1') = 206.25;</v>
+        <v>TX1(174,1) = 206.25;</v>
       </c>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B176" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(175,0') = 0.864999999999999;</v>
+        <v>TX1(175,0) = 0.864999999999999;</v>
       </c>
       <c r="C176">
         <f t="shared" si="10"/>
@@ -41441,15 +41440,15 @@
       <c r="F176">
         <v>210.9375</v>
       </c>
-      <c r="G176" t="str">
+      <c r="H176" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(175,1') = 210.9375;</v>
+        <v>TX1(175,1) = 210.9375;</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(176,0') = 0.864999999999999;</v>
+        <v>TX1(176,0) = 0.864999999999999;</v>
       </c>
       <c r="C177">
         <f t="shared" si="10"/>
@@ -41465,15 +41464,15 @@
       <c r="F177">
         <v>215.625</v>
       </c>
-      <c r="G177" t="str">
+      <c r="H177" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(176,1') = 215.625;</v>
+        <v>TX1(176,1) = 215.625;</v>
       </c>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B178" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(177,0') = 0.864999999999999;</v>
+        <v>TX1(177,0) = 0.864999999999999;</v>
       </c>
       <c r="C178">
         <f t="shared" si="10"/>
@@ -41489,15 +41488,15 @@
       <c r="F178">
         <v>220.3125</v>
       </c>
-      <c r="G178" t="str">
+      <c r="H178" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(177,1') = 220.3125;</v>
+        <v>TX1(177,1) = 220.3125;</v>
       </c>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B179" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(178,0') = 0.864999999999999;</v>
+        <v>TX1(178,0) = 0.864999999999999;</v>
       </c>
       <c r="C179">
         <f t="shared" si="10"/>
@@ -41513,15 +41512,15 @@
       <c r="F179">
         <v>225</v>
       </c>
-      <c r="G179" t="str">
+      <c r="H179" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(178,1') = 225;</v>
+        <v>TX1(178,1) = 225;</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B180" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(179,0') = 0.864999999999999;</v>
+        <v>TX1(179,0) = 0.864999999999999;</v>
       </c>
       <c r="C180">
         <f t="shared" si="10"/>
@@ -41537,15 +41536,15 @@
       <c r="F180">
         <v>229.6875</v>
       </c>
-      <c r="G180" t="str">
+      <c r="H180" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(179,1') = 229.6875;</v>
+        <v>TX1(179,1) = 229.6875;</v>
       </c>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B181" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(180,0') = 0.864999999999999;</v>
+        <v>TX1(180,0) = 0.864999999999999;</v>
       </c>
       <c r="C181">
         <f t="shared" si="10"/>
@@ -41561,15 +41560,15 @@
       <c r="F181">
         <v>234.375</v>
       </c>
-      <c r="G181" t="str">
+      <c r="H181" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(180,1') = 234.375;</v>
+        <v>TX1(180,1) = 234.375;</v>
       </c>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B182" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(181,0') = 0.864999999999999;</v>
+        <v>TX1(181,0) = 0.864999999999999;</v>
       </c>
       <c r="C182">
         <f t="shared" si="10"/>
@@ -41585,15 +41584,15 @@
       <c r="F182">
         <v>239.0625</v>
       </c>
-      <c r="G182" t="str">
+      <c r="H182" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(181,1') = 239.0625;</v>
+        <v>TX1(181,1) = 239.0625;</v>
       </c>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B183" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(182,0') = 0.864999999999999;</v>
+        <v>TX1(182,0) = 0.864999999999999;</v>
       </c>
       <c r="C183">
         <f t="shared" si="10"/>
@@ -41609,15 +41608,15 @@
       <c r="F183">
         <v>243.75</v>
       </c>
-      <c r="G183" t="str">
+      <c r="H183" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(182,1') = 243.75;</v>
+        <v>TX1(182,1) = 243.75;</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B184" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(183,0') = 0.864999999999999;</v>
+        <v>TX1(183,0) = 0.864999999999999;</v>
       </c>
       <c r="C184">
         <f t="shared" si="10"/>
@@ -41633,15 +41632,15 @@
       <c r="F184">
         <v>248.4375</v>
       </c>
-      <c r="G184" t="str">
+      <c r="H184" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(183,1') = 248.4375;</v>
+        <v>TX1(183,1) = 248.4375;</v>
       </c>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B185" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(184,0') = 0.864999999999999;</v>
+        <v>TX1(184,0) = 0.864999999999999;</v>
       </c>
       <c r="C185">
         <f t="shared" si="10"/>
@@ -41657,15 +41656,15 @@
       <c r="F185">
         <v>253.125</v>
       </c>
-      <c r="G185" t="str">
+      <c r="H185" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(184,1') = 253.125;</v>
+        <v>TX1(184,1) = 253.125;</v>
       </c>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B186" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(185,0') = 0.864999999999999;</v>
+        <v>TX1(185,0) = 0.864999999999999;</v>
       </c>
       <c r="C186">
         <f t="shared" si="10"/>
@@ -41681,15 +41680,15 @@
       <c r="F186">
         <v>257.8125</v>
       </c>
-      <c r="G186" t="str">
+      <c r="H186" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(185,1') = 257.8125;</v>
+        <v>TX1(185,1) = 257.8125;</v>
       </c>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B187" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(186,0') = 0.864999999999999;</v>
+        <v>TX1(186,0) = 0.864999999999999;</v>
       </c>
       <c r="C187">
         <f t="shared" si="10"/>
@@ -41705,15 +41704,15 @@
       <c r="F187">
         <v>262.5</v>
       </c>
-      <c r="G187" t="str">
+      <c r="H187" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(186,1') = 262.5;</v>
+        <v>TX1(186,1) = 262.5;</v>
       </c>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B188" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(187,0') = 0.864999999999999;</v>
+        <v>TX1(187,0) = 0.864999999999999;</v>
       </c>
       <c r="C188">
         <f t="shared" si="10"/>
@@ -41729,15 +41728,15 @@
       <c r="F188">
         <v>267.1875</v>
       </c>
-      <c r="G188" t="str">
+      <c r="H188" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(187,1') = 267.1875;</v>
+        <v>TX1(187,1) = 267.1875;</v>
       </c>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B189" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(188,0') = 0.864999999999999;</v>
+        <v>TX1(188,0) = 0.864999999999999;</v>
       </c>
       <c r="C189">
         <f t="shared" si="10"/>
@@ -41753,15 +41752,15 @@
       <c r="F189">
         <v>271.875</v>
       </c>
-      <c r="G189" t="str">
+      <c r="H189" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(188,1') = 271.875;</v>
+        <v>TX1(188,1) = 271.875;</v>
       </c>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B190" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(189,0') = 0.864999999999999;</v>
+        <v>TX1(189,0) = 0.864999999999999;</v>
       </c>
       <c r="C190">
         <f t="shared" si="10"/>
@@ -41777,15 +41776,15 @@
       <c r="F190">
         <v>276.5625</v>
       </c>
-      <c r="G190" t="str">
+      <c r="H190" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(189,1') = 276.5625;</v>
+        <v>TX1(189,1) = 276.5625;</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B191" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(190,0') = 0.864999999999999;</v>
+        <v>TX1(190,0) = 0.864999999999999;</v>
       </c>
       <c r="C191">
         <f t="shared" si="10"/>
@@ -41801,15 +41800,15 @@
       <c r="F191">
         <v>281.25</v>
       </c>
-      <c r="G191" t="str">
+      <c r="H191" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(190,1') = 281.25;</v>
+        <v>TX1(190,1) = 281.25;</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B192" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(191,0') = 0.864999999999999;</v>
+        <v>TX1(191,0) = 0.864999999999999;</v>
       </c>
       <c r="C192">
         <f t="shared" si="10"/>
@@ -41825,15 +41824,15 @@
       <c r="F192">
         <v>285.9375</v>
       </c>
-      <c r="G192" t="str">
+      <c r="H192" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(191,1') = 285.9375;</v>
+        <v>TX1(191,1) = 285.9375;</v>
       </c>
     </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B193" t="str">
         <f t="shared" si="8"/>
-        <v>TX1(192,0') = 0.864999999999999;</v>
+        <v>TX1(192,0) = 0.864999999999999;</v>
       </c>
       <c r="C193">
         <f t="shared" si="10"/>
@@ -41849,15 +41848,15 @@
       <c r="F193">
         <v>290.625</v>
       </c>
-      <c r="G193" t="str">
+      <c r="H193" t="str">
         <f t="shared" si="9"/>
-        <v>TX1(192,1') = 290.625;</v>
+        <v>TX1(192,1) = 290.625;</v>
       </c>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B194" t="str">
-        <f>_xlfn.CONCAT("TX1(",C194,",0","') = ",E194,";")</f>
-        <v>TX1(193,0') = 0.864999999999999;</v>
+        <f t="shared" ref="B194" si="12">_xlfn.CONCAT("TX1(",C194,",0",") = ",E194,";")</f>
+        <v>TX1(193,0) = 0.864999999999999;</v>
       </c>
       <c r="C194">
         <f t="shared" si="10"/>
@@ -41873,15 +41872,15 @@
       <c r="F194">
         <v>295.3125</v>
       </c>
-      <c r="G194" t="str">
-        <f>_xlfn.CONCAT("TX1(",C194,",1","') = ",F194,";")</f>
-        <v>TX1(193,1') = 295.3125;</v>
+      <c r="H194" t="str">
+        <f t="shared" ref="H194:H195" si="13">_xlfn.CONCAT("TX1(",C194,",1",") = ",F194,";")</f>
+        <v>TX1(193,1) = 295.3125;</v>
       </c>
     </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B195" t="str">
-        <f>_xlfn.CONCAT("TX1(",C195,",0","') = ",E195,";")</f>
-        <v>TX1(194,0') = 0.864999999999999;</v>
+        <f>_xlfn.CONCAT("TX1(",C195,",0",") = ",E195,";")</f>
+        <v>TX1(194,0) = 0.864999999999999;</v>
       </c>
       <c r="C195">
         <f>C194+1</f>
@@ -41897,9 +41896,9 @@
       <c r="F195">
         <v>300</v>
       </c>
-      <c r="G195" t="str">
-        <f>_xlfn.CONCAT("TX1(",C195,",1","') = ",F195,";")</f>
-        <v>TX1(194,1') = 300;</v>
+      <c r="H195" t="str">
+        <f t="shared" si="13"/>
+        <v>TX1(194,1) = 300;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>